<commit_message>
Add the list of asset with check
</commit_message>
<xml_diff>
--- a/Concept_Art/ConceptArt_ConceptAssets_ListToCheck_v01_011817.xlsx
+++ b/Concept_Art/ConceptArt_ConceptAssets_ListToCheck_v01_011817.xlsx
@@ -60,7 +60,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +73,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -155,13 +161,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +451,7 @@
   <dimension ref="B4:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,16 +461,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -478,25 +484,25 @@
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>